<commit_message>
Update AN-method output (no mundist).xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/AN-method output (no mundist).xlsx
+++ b/migforecasting/clustering/AN-method output (no mundist).xlsx
@@ -9,64 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="1" r:id="rId1"/>
+    <sheet name="Прогноз" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Анализ!$C$24:$R$24</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Анализ!$C$25:$R$25</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Анализ!$C$27:$R$27</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Анализ!$C$28:$R$28</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Анализ!$C$29:$R$29</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Анализ!$C$30:$R$30</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Анализ!$C$24:$R$24</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Анализ!$C$25:$R$25</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Анализ!$C$26:$R$26</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Анализ!$C$27:$R$27</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Анализ!$C$28:$R$28</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Анализ!$C$29:$R$29</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Анализ!$C$26:$R$26</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Анализ!$C$30:$R$30</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Анализ!$C$24:$R$24</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Анализ!$C$25:$R$25</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Анализ!$C$26:$R$26</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Анализ!$C$27:$R$27</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Анализ!$C$28:$R$28</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Анализ!$C$29:$R$29</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Анализ!$C$30:$R$30</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Анализ!$C$24:$R$24</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Анализ!$C$25:$R$25</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Анализ!$C$27:$R$27</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Анализ!$C$26:$R$26</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Анализ!$C$27:$R$27</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Анализ!$C$28:$R$28</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Анализ!$C$29:$R$29</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Анализ!$C$30:$R$30</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Анализ!$C$24:$R$24</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Анализ!$C$25:$R$25</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Анализ!$C$26:$R$26</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Анализ!$C$27:$R$27</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Анализ!$C$28:$R$28</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Анализ!$C$28:$R$28</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Анализ!$C$29:$R$29</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Анализ!$C$30:$R$30</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Анализ!$C$29:$R$29</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Анализ!$C$30:$R$30</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Анализ!$C$24:$R$24</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Анализ!$C$25:$R$25</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Анализ!$C$26:$R$26</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="27">
   <si>
     <t>clust</t>
   </si>
@@ -130,6 +87,24 @@
   <si>
     <t>avg</t>
   </si>
+  <si>
+    <t>Процент превосходства соцэко индикатора в положительной части кластера по сравнению с отрицательной</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>neg+pos</t>
+  </si>
+  <si>
+    <t>pred saldo</t>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +114,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +149,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -240,6 +224,19 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1357,7 +1354,7 @@
             <c:numRef>
               <c:f>[1]Анализ!$D$25:$R$25</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>-4.5743197755307441E-2</c:v>
@@ -1486,7 +1483,7 @@
             <c:numRef>
               <c:f>[1]Анализ!$D$26:$R$26</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>3.0509624868235496E-2</c:v>
@@ -1615,7 +1612,7 @@
             <c:numRef>
               <c:f>[1]Анализ!$D$27:$R$27</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>-9.276436666696275E-2</c:v>
@@ -1744,7 +1741,7 @@
             <c:numRef>
               <c:f>[1]Анализ!$D$28:$R$28</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>-8.8491683697801138E-3</c:v>
@@ -1873,7 +1870,7 @@
             <c:numRef>
               <c:f>[1]Анализ!$D$29:$R$29</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>-1.0808853999729751E-3</c:v>
@@ -2002,7 +1999,7 @@
             <c:numRef>
               <c:f>[1]Анализ!$D$30:$R$30</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>-8.3641311857414191E-2</c:v>
@@ -2152,7 +2149,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3788,7 +3785,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4081,8 +4078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4942,6 +4939,11 @@
         <v>19</v>
       </c>
     </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H23" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C24" s="7" t="s">
         <v>2</v>
@@ -5417,67 +5419,67 @@
         <v>20</v>
       </c>
       <c r="C31" s="9">
-        <f>AVERAGE(C25:C30)</f>
+        <f t="shared" ref="C31:I31" si="7">AVERAGE(C25:C30)</f>
         <v>0.1530882296273029</v>
       </c>
       <c r="D31" s="9">
-        <f>AVERAGE(D25:D30)</f>
+        <f t="shared" si="7"/>
         <v>-4.3158937537187657E-2</v>
       </c>
       <c r="E31" s="9">
-        <f>AVERAGE(E25:E30)</f>
+        <f t="shared" si="7"/>
         <v>4.3246496906242902E-2</v>
       </c>
       <c r="F31" s="9">
-        <f>AVERAGE(F25:F30)</f>
+        <f t="shared" si="7"/>
         <v>3.8713878631365585E-2</v>
       </c>
       <c r="G31" s="9">
-        <f>AVERAGE(G25:G30)</f>
+        <f t="shared" si="7"/>
         <v>0.17756314057400535</v>
       </c>
       <c r="H31" s="9">
-        <f>AVERAGE(H25:H30)</f>
+        <f t="shared" si="7"/>
         <v>0.22431998874260226</v>
       </c>
       <c r="I31" s="9">
-        <f>AVERAGE(I25:I30)</f>
+        <f t="shared" si="7"/>
         <v>2.0717030584713875E-2</v>
       </c>
       <c r="J31" s="9">
-        <f t="shared" ref="J31:R31" si="7">AVERAGE(J25:J30)</f>
+        <f t="shared" ref="J31:R31" si="8">AVERAGE(J25:J30)</f>
         <v>2.1836382204897253E-3</v>
       </c>
       <c r="K31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.2850431550950217E-3</v>
       </c>
       <c r="L31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-7.1040558569823622E-2</v>
       </c>
       <c r="M31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-3.4643133764610402E-2</v>
       </c>
       <c r="N31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.06504684645584E-2</v>
       </c>
       <c r="O31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.7002235654687617E-2</v>
       </c>
       <c r="P31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-2.851464442612241E-2</v>
       </c>
       <c r="Q31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-3.5058627549486278E-2</v>
       </c>
       <c r="R31" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-3.6035858668642083E-2</v>
       </c>
     </row>
@@ -6710,4 +6712,2782 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4">
+        <v>164807.99111111101</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.239321378776819</v>
+      </c>
+      <c r="E2" s="3">
+        <v>29018.855729342202</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.1510354114894401</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.7896575371105697E-2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>70.700341358427195</v>
+      </c>
+      <c r="I2" s="3">
+        <v>26.740573333333302</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2.0003527914307299E-3</v>
+      </c>
+      <c r="K2" s="3">
+        <v>3.5529138963616498E-3</v>
+      </c>
+      <c r="L2" s="3">
+        <v>2.5364955631528101E-3</v>
+      </c>
+      <c r="M2" s="3">
+        <v>8.8732967316838898E-2</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.21304175032453901</v>
+      </c>
+      <c r="O2" s="3">
+        <v>2.7362961348447499</v>
+      </c>
+      <c r="P2" s="6">
+        <v>3.6724036200784001E-4</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>5.7659091342652999E-2</v>
+      </c>
+      <c r="R2" s="3">
+        <v>264.58127835258301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4">
+        <v>131645.14432989599</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.246119353999494</v>
+      </c>
+      <c r="E3" s="3">
+        <v>27897.187580030899</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.2177236272124601</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.5632743956943498E-2</v>
+      </c>
+      <c r="H3" s="3">
+        <v>66.670508836377095</v>
+      </c>
+      <c r="I3" s="3">
+        <v>26.084737113401999</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2.20289984411654E-3</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3.6263849299225498E-3</v>
+      </c>
+      <c r="L3" s="3">
+        <v>3.2259364151279901E-3</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.102195588506201</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.220122066507287</v>
+      </c>
+      <c r="O3" s="3">
+        <v>2.7514922487599902</v>
+      </c>
+      <c r="P3" s="6">
+        <v>3.4140684121260098E-4</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>6.1164265955433401E-2</v>
+      </c>
+      <c r="R3" s="3">
+        <v>265.87990616144202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4">
+        <v>131645.14432989599</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.246119353999494</v>
+      </c>
+      <c r="E4" s="3">
+        <v>29018.855729342202</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.2177236272124601</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3.7896575371105697E-2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>70.700341358427195</v>
+      </c>
+      <c r="I4" s="3">
+        <v>26.740573333333302</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2.20289984411654E-3</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3.6263849299225498E-3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3.2259364151279901E-3</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.102195588506201</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.220122066507287</v>
+      </c>
+      <c r="O4" s="3">
+        <v>2.7514922487599902</v>
+      </c>
+      <c r="P4" s="6">
+        <v>3.6724036200784001E-4</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>6.1164265955433401E-2</v>
+      </c>
+      <c r="R4" s="3">
+        <v>265.87990616144202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4">
+        <v>72566.171521035605</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.189583292061173</v>
+      </c>
+      <c r="E7" s="3">
+        <v>23588.468394812298</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.78534973699159805</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2.6962929605903001E-2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>36.985917288836298</v>
+      </c>
+      <c r="I7" s="3">
+        <v>24.400728155339699</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2.0809070905413599E-3</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2.74273251356547E-3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>4.0126866040288501E-3</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.16115439742513701</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.26232777031080001</v>
+      </c>
+      <c r="O7" s="3">
+        <v>2.9265367600548799</v>
+      </c>
+      <c r="P7" s="6">
+        <v>1.8333715088117699E-4</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>5.2500220873737603E-2</v>
+      </c>
+      <c r="R7" s="3">
+        <v>160.88126020636</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4">
+        <v>73801.019762845797</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.209212442971625</v>
+      </c>
+      <c r="E8" s="3">
+        <v>23772.118956875402</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.78195361276530495</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.4549296075286602E-2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>34.278988580233801</v>
+      </c>
+      <c r="I8" s="3">
+        <v>24.7749644268774</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2.1654613025601601E-3</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2.8679616426797098E-3</v>
+      </c>
+      <c r="L8" s="3">
+        <v>4.2579877024096803E-3</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.16877386288204399</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.25906880817927902</v>
+      </c>
+      <c r="O8" s="3">
+        <v>3.40365018026902</v>
+      </c>
+      <c r="P8" s="6">
+        <v>1.9956967010239599E-4</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>5.5645145794321997E-2</v>
+      </c>
+      <c r="R8" s="3">
+        <v>168.31403626084099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4">
+        <v>73801.019762845797</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.209212442971625</v>
+      </c>
+      <c r="E9" s="3">
+        <v>23772.118956875402</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.78534973699159805</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.6962929605903001E-2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>36.985917288836298</v>
+      </c>
+      <c r="I9" s="3">
+        <v>24.7749644268774</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2.1654613025601601E-3</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2.8679616426797098E-3</v>
+      </c>
+      <c r="L9" s="3">
+        <v>4.2579877024096803E-3</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.16877386288204399</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.26232777031080001</v>
+      </c>
+      <c r="O9" s="3">
+        <v>3.40365018026902</v>
+      </c>
+      <c r="P9" s="6">
+        <v>1.9956967010239599E-4</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>5.5645145794321997E-2</v>
+      </c>
+      <c r="R9" s="3">
+        <v>168.31403626084099</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4">
+        <v>68564.535353535306</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.18660119189643201</v>
+      </c>
+      <c r="E12" s="3">
+        <v>27344.810889393899</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.696620980986972</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2.2582897619523999E-2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>35.027230891321203</v>
+      </c>
+      <c r="I12" s="3">
+        <v>26.9908787878787</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.8800419758275299E-3</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3.2827919550483101E-3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>5.81489591983531E-3</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0.34613357156156899</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.70788762087819801</v>
+      </c>
+      <c r="O12" s="3">
+        <v>9.6041584244655507</v>
+      </c>
+      <c r="P12" s="6">
+        <v>2.7891952968457401E-4</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>5.2421230906235898E-2</v>
+      </c>
+      <c r="R12" s="3">
+        <v>267.76056498903802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4">
+        <v>59076.652482269397</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.203789163958256</v>
+      </c>
+      <c r="E13" s="3">
+        <v>25467.048701702101</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.72689230178861897</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2.4085878336496599E-2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>28.1941841407913</v>
+      </c>
+      <c r="I13" s="3">
+        <v>26.5204822695035</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.9727956823579001E-3</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3.8442672703875198E-3</v>
+      </c>
+      <c r="L13" s="3">
+        <v>5.8133878270779501E-3</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0.295989957871853</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0.62134179787733601</v>
+      </c>
+      <c r="O13" s="3">
+        <v>8.4609746898260401</v>
+      </c>
+      <c r="P13" s="6">
+        <v>2.6764459457439399E-4</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>5.4713383918701002E-2</v>
+      </c>
+      <c r="R13" s="3">
+        <v>215.08277428894999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4">
+        <v>59076.652482269397</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.203789163958256</v>
+      </c>
+      <c r="E14" s="3">
+        <v>27344.810889393899</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.72689230178861897</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2.4085878336496599E-2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>35.027230891321203</v>
+      </c>
+      <c r="I14" s="3">
+        <v>26.9908787878787</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1.9727956823579001E-3</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3.8442672703875198E-3</v>
+      </c>
+      <c r="L14" s="3">
+        <v>5.81489591983531E-3</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.34613357156156899</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0.70788762087819801</v>
+      </c>
+      <c r="O14" s="3">
+        <v>9.6041584244655507</v>
+      </c>
+      <c r="P14" s="6">
+        <v>2.7891952968457401E-4</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>5.4713383918701002E-2</v>
+      </c>
+      <c r="R14" s="3">
+        <v>267.76056498903802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="4">
+        <v>111014.81372549001</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.32683220031052201</v>
+      </c>
+      <c r="E17" s="3">
+        <v>41503.168199941101</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.815226802093581</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3.24414268916191E-2</v>
+      </c>
+      <c r="H17" s="3">
+        <v>54.825693016465202</v>
+      </c>
+      <c r="I17" s="3">
+        <v>23.593235294117601</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2.2292113632206901E-3</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3.2357838718698501E-3</v>
+      </c>
+      <c r="L17" s="3">
+        <v>2.3894848550633798E-3</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0.125021890782716</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0.22367674443591101</v>
+      </c>
+      <c r="O17" s="3">
+        <v>2.86389544791649</v>
+      </c>
+      <c r="P17" s="6">
+        <v>2.6414080743661101E-4</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>6.0080075813557503E-2</v>
+      </c>
+      <c r="R17" s="3">
+        <v>814.51301889204206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="4">
+        <v>88443.299578058999</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.305918761473154</v>
+      </c>
+      <c r="E18" s="3">
+        <v>38241.899439367102</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.82108311154265501</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2.84526948642621E-2</v>
+      </c>
+      <c r="H18" s="3">
+        <v>43.740974774376497</v>
+      </c>
+      <c r="I18" s="3">
+        <v>24.495864978902901</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2.1840552471381999E-3</v>
+      </c>
+      <c r="K18" s="3">
+        <v>3.0631903056150098E-3</v>
+      </c>
+      <c r="L18" s="3">
+        <v>2.76036340572282E-3</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.17655458040053501</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0.23098281618261399</v>
+      </c>
+      <c r="O18" s="3">
+        <v>2.8729539348869002</v>
+      </c>
+      <c r="P18" s="6">
+        <v>2.6245664983897299E-4</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>6.3919879791429296E-2</v>
+      </c>
+      <c r="R18" s="3">
+        <v>814.86215366019201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4">
+        <v>88443.299578058999</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.32683220031052201</v>
+      </c>
+      <c r="E19" s="3">
+        <v>41503.168199941101</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.82108311154265501</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3.24414268916191E-2</v>
+      </c>
+      <c r="H19" s="3">
+        <v>54.825693016465202</v>
+      </c>
+      <c r="I19" s="3">
+        <v>24.495864978902901</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2.2292113632206901E-3</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3.2357838718698501E-3</v>
+      </c>
+      <c r="L19" s="3">
+        <v>2.76036340572282E-3</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.17655458040053501</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0.23098281618261399</v>
+      </c>
+      <c r="O19" s="3">
+        <v>2.8729539348869002</v>
+      </c>
+      <c r="P19" s="6">
+        <v>2.6414080743661101E-4</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>6.3919879791429296E-2</v>
+      </c>
+      <c r="R19" s="3">
+        <v>814.86215366019201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4">
+        <v>34346.433333333298</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.21496354724112501</v>
+      </c>
+      <c r="E22" s="3">
+        <v>26552.813493666599</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.86251438707031902</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2.4400277185926401E-2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>44.121309838155902</v>
+      </c>
+      <c r="I22" s="3">
+        <v>29.957666666666601</v>
+      </c>
+      <c r="J22" s="3">
+        <v>3.2810787544048899E-3</v>
+      </c>
+      <c r="K22" s="3">
+        <v>2.7291930340570402E-3</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1.35377439196805E-2</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0.47448492008406401</v>
+      </c>
+      <c r="N22" s="3">
+        <v>0.40599525933667702</v>
+      </c>
+      <c r="O22" s="3">
+        <v>12.534415451913601</v>
+      </c>
+      <c r="P22" s="6">
+        <v>5.7502760830474499E-4</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>6.06464201617491E-2</v>
+      </c>
+      <c r="R22" s="3">
+        <v>272.65362399689297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>4</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4">
+        <v>26444.322033898199</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.21952941930022701</v>
+      </c>
+      <c r="E23" s="3">
+        <v>24460.203132033799</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.78617270372581005</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2.5920375933912901E-2</v>
+      </c>
+      <c r="H23" s="3">
+        <v>36.6974660118399</v>
+      </c>
+      <c r="I23" s="3">
+        <v>29.721847457627099</v>
+      </c>
+      <c r="J23" s="3">
+        <v>3.1768415513344001E-3</v>
+      </c>
+      <c r="K23" s="3">
+        <v>2.5529049066565501E-3</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1.56201208189133E-2</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.38505660479326298</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0.321434376034967</v>
+      </c>
+      <c r="O23" s="3">
+        <v>8.7696547847163107</v>
+      </c>
+      <c r="P23" s="6">
+        <v>5.8060175953319202E-4</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>5.94341737712809E-2</v>
+      </c>
+      <c r="R23" s="3">
+        <v>255.66572324290701</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>4</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="4">
+        <v>26444.322033898199</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.21952941930022701</v>
+      </c>
+      <c r="E24" s="3">
+        <v>26552.813493666599</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.86251438707031902</v>
+      </c>
+      <c r="G24" s="3">
+        <v>2.5920375933912901E-2</v>
+      </c>
+      <c r="H24" s="3">
+        <v>44.121309838155902</v>
+      </c>
+      <c r="I24" s="3">
+        <v>29.957666666666601</v>
+      </c>
+      <c r="J24" s="3">
+        <v>3.2810787544048899E-3</v>
+      </c>
+      <c r="K24" s="3">
+        <v>2.7291930340570402E-3</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1.56201208189133E-2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0.47448492008406401</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0.40599525933667702</v>
+      </c>
+      <c r="O24" s="3">
+        <v>12.534415451913601</v>
+      </c>
+      <c r="P24" s="6">
+        <v>5.8060175953319202E-4</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>6.06464201617491E-2</v>
+      </c>
+      <c r="R24" s="3">
+        <v>272.65362399689297</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>5</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="4">
+        <v>31693.882352941098</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.15488522798111401</v>
+      </c>
+      <c r="E27" s="3">
+        <v>21673.311809411702</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.79009004932782401</v>
+      </c>
+      <c r="G27" s="3">
+        <v>3.17925233079384E-2</v>
+      </c>
+      <c r="H27" s="3">
+        <v>40.805636315725103</v>
+      </c>
+      <c r="I27" s="3">
+        <v>30.596588235294099</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2.8423504392595298E-3</v>
+      </c>
+      <c r="K27" s="3">
+        <v>2.3967383316014701E-3</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1.6617257829695101E-2</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.81707199487590298</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0.75702905721362301</v>
+      </c>
+      <c r="O27" s="3">
+        <v>22.535907071104901</v>
+      </c>
+      <c r="P27" s="6">
+        <v>5.6204664330488903E-4</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>5.6296507891859797E-2</v>
+      </c>
+      <c r="R27" s="3">
+        <v>86.674616944433694</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>5</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="4">
+        <v>32717.342857142801</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.17223464862844801</v>
+      </c>
+      <c r="E28" s="3">
+        <v>22060.863952571399</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.64007213047926503</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1.6871552770673402E-2</v>
+      </c>
+      <c r="H28" s="3">
+        <v>27.051620347179401</v>
+      </c>
+      <c r="I28" s="3">
+        <v>27.186285714285699</v>
+      </c>
+      <c r="J28" s="3">
+        <v>2.4984980007264901E-3</v>
+      </c>
+      <c r="K28" s="3">
+        <v>2.1018633936642E-3</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1.49368977269919E-2</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.950919980446152</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0.70568554871173805</v>
+      </c>
+      <c r="O28" s="3">
+        <v>22.845238599246301</v>
+      </c>
+      <c r="P28" s="6">
+        <v>7.0640901064990096E-4</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>5.7151331170984601E-2</v>
+      </c>
+      <c r="R28" s="3">
+        <v>166.077274161171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>5</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="4">
+        <v>32717.342857142801</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.17223464862844801</v>
+      </c>
+      <c r="E29" s="3">
+        <v>22060.863952571399</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.79009004932782401</v>
+      </c>
+      <c r="G29" s="3">
+        <v>3.17925233079384E-2</v>
+      </c>
+      <c r="H29" s="3">
+        <v>40.805636315725103</v>
+      </c>
+      <c r="I29" s="3">
+        <v>30.596588235294099</v>
+      </c>
+      <c r="J29" s="3">
+        <v>2.8423504392595298E-3</v>
+      </c>
+      <c r="K29" s="3">
+        <v>2.3967383316014701E-3</v>
+      </c>
+      <c r="L29" s="3">
+        <v>1.6617257829695101E-2</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0.950919980446152</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0.75702905721362301</v>
+      </c>
+      <c r="O29" s="3">
+        <v>22.845238599246301</v>
+      </c>
+      <c r="P29" s="6">
+        <v>7.0640901064990096E-4</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>5.7151331170984601E-2</v>
+      </c>
+      <c r="R29" s="3">
+        <v>166.077274161171</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="colorScale" priority="237">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D3">
+    <cfRule type="colorScale" priority="236">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E3">
+    <cfRule type="colorScale" priority="235">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F3">
+    <cfRule type="colorScale" priority="234">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G3">
+    <cfRule type="colorScale" priority="233">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H3">
+    <cfRule type="colorScale" priority="232">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I3">
+    <cfRule type="colorScale" priority="231">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J3">
+    <cfRule type="colorScale" priority="230">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K3">
+    <cfRule type="colorScale" priority="229">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L3">
+    <cfRule type="colorScale" priority="228">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M3">
+    <cfRule type="colorScale" priority="227">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N3">
+    <cfRule type="colorScale" priority="226">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O3">
+    <cfRule type="colorScale" priority="225">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P3">
+    <cfRule type="colorScale" priority="224">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q3">
+    <cfRule type="colorScale" priority="223">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R3">
+    <cfRule type="colorScale" priority="222">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="colorScale" priority="205">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="colorScale" priority="204">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="colorScale" priority="203">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="colorScale" priority="202">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4">
+    <cfRule type="colorScale" priority="201">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:C8">
+    <cfRule type="colorScale" priority="200">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:D8">
+    <cfRule type="colorScale" priority="199">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E8">
+    <cfRule type="colorScale" priority="198">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:F8">
+    <cfRule type="colorScale" priority="197">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:G8">
+    <cfRule type="colorScale" priority="196">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:H8">
+    <cfRule type="colorScale" priority="195">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:I8">
+    <cfRule type="colorScale" priority="194">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:J8">
+    <cfRule type="colorScale" priority="193">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7:K8">
+    <cfRule type="colorScale" priority="192">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7:L8">
+    <cfRule type="colorScale" priority="191">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7:M8">
+    <cfRule type="colorScale" priority="190">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:N8">
+    <cfRule type="colorScale" priority="189">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7:O8">
+    <cfRule type="colorScale" priority="188">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P7:P8">
+    <cfRule type="colorScale" priority="187">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q7:Q8">
+    <cfRule type="colorScale" priority="186">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7:R8">
+    <cfRule type="colorScale" priority="185">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="colorScale" priority="168">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="colorScale" priority="167">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="colorScale" priority="166">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9">
+    <cfRule type="colorScale" priority="165">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:C13">
+    <cfRule type="colorScale" priority="164">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D13">
+    <cfRule type="colorScale" priority="163">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E13">
+    <cfRule type="colorScale" priority="162">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F13">
+    <cfRule type="colorScale" priority="161">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G13">
+    <cfRule type="colorScale" priority="160">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H13">
+    <cfRule type="colorScale" priority="159">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:I13">
+    <cfRule type="colorScale" priority="158">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12:J13">
+    <cfRule type="colorScale" priority="157">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12:K13">
+    <cfRule type="colorScale" priority="156">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12:L13">
+    <cfRule type="colorScale" priority="155">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12:M13">
+    <cfRule type="colorScale" priority="154">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N12:N13">
+    <cfRule type="colorScale" priority="153">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O12:O13">
+    <cfRule type="colorScale" priority="152">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P12:P13">
+    <cfRule type="colorScale" priority="151">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q12:Q13">
+    <cfRule type="colorScale" priority="150">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R12:R13">
+    <cfRule type="colorScale" priority="149">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="colorScale" priority="131">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="colorScale" priority="130">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="colorScale" priority="129">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="colorScale" priority="128">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M14">
+    <cfRule type="colorScale" priority="127">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N14">
+    <cfRule type="colorScale" priority="126">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O14">
+    <cfRule type="colorScale" priority="125">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14">
+    <cfRule type="colorScale" priority="124">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R14">
+    <cfRule type="colorScale" priority="123">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:C18">
+    <cfRule type="colorScale" priority="122">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:D18">
+    <cfRule type="colorScale" priority="121">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:E18">
+    <cfRule type="colorScale" priority="120">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17:F18">
+    <cfRule type="colorScale" priority="119">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:G18">
+    <cfRule type="colorScale" priority="118">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:H18">
+    <cfRule type="colorScale" priority="117">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17:I18">
+    <cfRule type="colorScale" priority="116">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17:J18">
+    <cfRule type="colorScale" priority="115">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17:K18">
+    <cfRule type="colorScale" priority="114">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17:L18">
+    <cfRule type="colorScale" priority="113">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:M18">
+    <cfRule type="colorScale" priority="112">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N17:N18">
+    <cfRule type="colorScale" priority="111">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:O18">
+    <cfRule type="colorScale" priority="110">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P17:P18">
+    <cfRule type="colorScale" priority="109">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17:Q18">
+    <cfRule type="colorScale" priority="108">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R17:R18">
+    <cfRule type="colorScale" priority="107">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="colorScale" priority="90">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="colorScale" priority="89">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
+    <cfRule type="colorScale" priority="88">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="colorScale" priority="85">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P19">
+    <cfRule type="colorScale" priority="84">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C23">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D23">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E23">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F23">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:G23">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:H23">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:I23">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22:J23">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22:K23">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L22:L23">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M22:M23">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N22:N23">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O22:O23">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P22:P23">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q22:Q23">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R22:R23">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M24">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N24">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O24">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q24">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R24">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:C28">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:D28">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:E28">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:F28">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27:G28">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:H28">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27:I28">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J27:J28">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27:K28">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L27:L28">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M27:M28">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N27:N28">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O27:O28">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P27:P28">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q27:Q28">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R27:R28">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L29">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>